<commit_message>
8 and 9 commit
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JAVA ECLIPSE\40 day data Structure Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A056988-25B9-4A1E-8C27-67048FF22C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD44C421-4EE0-4AE0-8E3D-1177CF3D8641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="323">
   <si>
     <t>#CrackYourInternship</t>
   </si>
@@ -1488,8 +1488,8 @@
   </sheetPr>
   <dimension ref="A1:I333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1885,6 +1885,9 @@
       <c r="C37" s="9" t="s">
         <v>43</v>
       </c>
+      <c r="D37" t="s">
+        <v>322</v>
+      </c>
       <c r="H37" s="10" t="s">
         <v>13</v>
       </c>
@@ -1904,6 +1907,9 @@
       <c r="C39" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="D39" t="s">
+        <v>322</v>
+      </c>
       <c r="H39" s="10" t="s">
         <v>13</v>
       </c>
@@ -1914,6 +1920,9 @@
       </c>
       <c r="C40" s="9" t="s">
         <v>46</v>
+      </c>
+      <c r="D40" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="13.2">

</xml_diff>